<commit_message>
bug fixed in Python and translated to c++
</commit_message>
<xml_diff>
--- a/namen.xlsx
+++ b/namen.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>